<commit_message>
Changed the survey_data.xlsx file to a tidy format and saved it as a .csv file
</commit_message>
<xml_diff>
--- a/messy-project-directory/data/survey_data.xlsx
+++ b/messy-project-directory/data/survey_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/shaffman_uw_edu/Documents/Documents/Classes/Tools in Computational Biology/homework01/messy-project-directory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FF08295-EDB6-4FB6-9984-33B70EB27BC7}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54495" yWindow="-5340" windowWidth="26010" windowHeight="20985" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="38">
   <si>
     <t>NA</t>
   </si>
@@ -121,25 +121,28 @@
     <t>Plot: 4</t>
   </si>
   <si>
-    <t>species_sex</t>
-  </si>
-  <si>
     <t>wgt</t>
   </si>
   <si>
-    <t>DM_F</t>
-  </si>
-  <si>
-    <t>DM_M</t>
-  </si>
-  <si>
-    <t>DO_M</t>
-  </si>
-  <si>
-    <t>OL_M</t>
-  </si>
-  <si>
-    <t>gray cell means my measurement device wasn't calibrated correctly</t>
+    <t xml:space="preserve">157 scale no calibrated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">218 Scale not Calibrated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">species </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>OL</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,7 +337,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -731,7 +733,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,7 +777,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -800,30 +802,30 @@
   <dimension ref="C3:AB28"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="C5" sqref="C5:P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1"/>
-    <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" customWidth="1"/>
-    <col min="16" max="16" width="52.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="26.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="16" max="16" width="52.85546875" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
-    <col min="26" max="26" width="17.5" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="1"/>
+    <col min="20" max="20" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="19.85546875" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" customWidth="1"/>
+    <col min="29" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" ht="79" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" ht="78.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C3" s="11" t="s">
         <v>20</v>
       </c>
@@ -842,7 +844,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -859,7 +861,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -876,7 +878,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
@@ -899,298 +901,298 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="5">
         <v>2</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1201,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.4">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1238,7 +1240,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1255,7 +1257,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1272,7 +1274,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1289,7 +1291,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1306,7 +1308,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1323,7 +1325,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1340,7 +1342,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1357,7 +1359,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1366,7 +1368,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1375,22 +1377,22 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G25" s="5"/>
       <c r="L25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G26" s="5"/>
       <c r="L26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G27" s="5"/>
       <c r="L27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G28" s="5"/>
       <c r="L28" s="5"/>
       <c r="Q28" s="5"/>
@@ -1411,28 +1413,28 @@
   <dimension ref="C2:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="C6" sqref="C6:R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" style="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
-    <col min="15" max="19" width="11.5" style="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="22.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
+    <col min="15" max="19" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1455,7 +1457,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1498,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C8" s="6">
         <v>41648</v>
       </c>
@@ -1533,7 +1535,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C9" s="6">
         <v>41648</v>
       </c>
@@ -1572,7 +1574,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C10" s="6">
         <v>41711</v>
       </c>
@@ -1607,7 +1609,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C11" s="6">
         <v>41711</v>
       </c>
@@ -1648,7 +1650,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C12" s="6">
         <v>41711</v>
       </c>
@@ -1685,7 +1687,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1700,8 +1702,8 @@
       <c r="J13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="10">
-        <v>157</v>
+      <c r="K13" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="7">
@@ -1718,7 +1720,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1747,7 +1749,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1762,8 +1764,8 @@
       <c r="J15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="10">
-        <v>218</v>
+      <c r="K15" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1772,7 +1774,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1797,7 +1799,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1822,7 +1824,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1839,7 +1841,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1856,7 +1858,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1873,7 +1875,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1890,16 +1892,14 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:17" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="I22" s="9"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1909,7 +1909,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1926,7 +1926,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1943,7 +1943,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1960,7 +1960,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1977,7 +1977,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1996,17 +1996,19 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2019,17 +2021,19 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C29" s="6">
         <v>28498</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4">
         <v>37</v>
       </c>
-      <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2042,15 +2046,17 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C30" s="6">
         <v>28498</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2063,17 +2069,19 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C31" s="6">
         <v>28498</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="4">
         <v>48</v>
       </c>
-      <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2086,17 +2094,19 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C32" s="6">
         <v>28498</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="4">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4">
         <v>52</v>
       </c>
-      <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -2109,17 +2119,19 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C33" s="6">
         <v>28498</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
         <v>35</v>
       </c>
-      <c r="E33" s="4">
-        <v>35</v>
-      </c>
-      <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2132,7 +2144,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2149,7 +2161,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2166,7 +2178,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2183,7 +2195,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2198,7 +2210,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2215,7 +2227,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="L39" s="5"/>
@@ -2225,7 +2237,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="L40" s="5"/>
@@ -2235,7 +2247,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="L41" s="5"/>
@@ -2245,34 +2257,34 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="L42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="L43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G44" s="5"/>
       <c r="L44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G45" s="5"/>
       <c r="L45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G46" s="5"/>
       <c r="L46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G47" s="5"/>
       <c r="L47" s="5"/>
       <c r="Q47" s="5"/>

</xml_diff>